<commit_message>
make a new project -- a spider get data from dhgate --
</commit_message>
<xml_diff>
--- a/Work App/epacket.xlsx
+++ b/Work App/epacket.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="16980" windowHeight="10950" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="10950" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="standard" sheetId="1" r:id="rId1"/>
+    <sheet name="discount" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="44">
   <si>
     <t>country</t>
   </si>
@@ -42,7 +42,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>us,usa,united states,american,</t>
     </r>
@@ -60,7 +60,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>au,australia,</t>
     </r>
@@ -78,7 +78,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>uk,united kingdom,</t>
     </r>
@@ -96,7 +96,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>il,israel,</t>
     </r>
@@ -114,7 +114,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>fr,france,</t>
     </r>
@@ -132,7 +132,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>ca,canada,</t>
     </r>
@@ -150,7 +150,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>no,norway,</t>
     </r>
@@ -168,7 +168,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>sa,saudi arabia,</t>
     </r>
@@ -186,7 +186,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>ua,ukraine,</t>
     </r>
@@ -204,7 +204,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>de,germany,</t>
     </r>
@@ -222,7 +222,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>br,brazil,</t>
     </r>
@@ -240,7 +240,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>ru,russian federation,</t>
     </r>
@@ -258,7 +258,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>nz,new zealand,</t>
     </r>
@@ -276,7 +276,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>jp,japan,</t>
     </r>
@@ -294,7 +294,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>hk,hong kong,</t>
     </r>
@@ -325,7 +325,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>my,malaysia,</t>
     </r>
@@ -343,7 +343,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>sg,singapore,</t>
     </r>
@@ -361,7 +361,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>tr,turkey,</t>
     </r>
@@ -379,7 +379,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>at,austria,</t>
     </r>
@@ -397,7 +397,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>be,belgium,</t>
     </r>
@@ -415,7 +415,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>ch,switzerland,</t>
     </r>
@@ -433,7 +433,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>dk,denmark,</t>
     </r>
@@ -451,7 +451,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>hu,hungary,</t>
     </r>
@@ -469,7 +469,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>it,italy,</t>
     </r>
@@ -487,7 +487,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>lu,luxembourg,</t>
     </r>
@@ -505,7 +505,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>nl,netherlands,</t>
     </r>
@@ -523,7 +523,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>pl,poland,</t>
     </r>
@@ -541,7 +541,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>se,sweden,</t>
     </r>
@@ -559,7 +559,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>fl,finland,</t>
     </r>
@@ -577,7 +577,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>ie,ireland,</t>
     </r>
@@ -595,7 +595,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>pt,portugal,</t>
     </r>
@@ -613,7 +613,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>mx,mexico,</t>
     </r>
@@ -631,19 +631,25 @@
   </si>
   <si>
     <t>th,thiland,泰国</t>
+  </si>
+  <si>
+    <t>weight</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>discount</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -652,359 +658,23 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="9"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1012,295 +682,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1386,7 +782,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CCE8CF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1630,25 +1026,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.5" customWidth="1"/>
-    <col min="2" max="1025" width="10.9583333333333" customWidth="1"/>
+    <col min="2" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1671,7 +1067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1682,19 +1078,19 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.076</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2">
-        <v>0.076</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1717,7 +1113,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1734,13 +1130,13 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="G4">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1763,7 +1159,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1786,7 +1182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1803,13 +1199,13 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="G7">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1826,13 +1222,13 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="G8">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1855,7 +1251,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1866,19 +1262,19 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1901,7 +1297,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1924,7 +1320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1935,19 +1331,19 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0.092</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="E13">
         <v>8</v>
       </c>
       <c r="F13">
-        <v>0.092</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="G13">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1958,19 +1354,19 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E14">
         <v>9</v>
       </c>
       <c r="F14">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G14">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1993,7 +1389,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -2016,7 +1412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -2039,7 +1435,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -2056,13 +1452,13 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G18">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -2079,13 +1475,13 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G19">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -2108,7 +1504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -2131,7 +1527,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -2154,7 +1550,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -2177,7 +1573,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -2200,7 +1596,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -2223,7 +1619,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -2246,7 +1642,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -2269,7 +1665,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -2292,7 +1688,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -2315,7 +1711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -2338,7 +1734,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
@@ -2355,13 +1751,13 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="G31">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
@@ -2378,13 +1774,13 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="G32">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
@@ -2401,13 +1797,13 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="G33">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -2430,7 +1826,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -2453,7 +1849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2470,18 +1866,1414 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G36">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12页 &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C125"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>250</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>350</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>400</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>300</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>350</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>400</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>450</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>500</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>250</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>300</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>400</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>500</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>400</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>500</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>600</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1">
+        <v>700</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1">
+        <v>350</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1">
+        <v>400</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="1">
+        <v>500</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="1">
+        <v>600</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="1">
+        <v>650</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1">
+        <v>200</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1">
+        <v>300</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1">
+        <v>400</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1">
+        <v>450</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>350</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1">
+        <v>400</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="1">
+        <v>450</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="1">
+        <v>200</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>300</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="1">
+        <v>250</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="1">
+        <v>300</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <v>400</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="1">
+        <v>500</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="1">
+        <v>600</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>300</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40">
+        <v>150</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41">
+        <v>200</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42">
+        <v>300</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43">
+        <v>400</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44">
+        <v>450</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.91500000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45">
+        <v>250</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>300</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47">
+        <v>200</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48">
+        <v>300</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49">
+        <v>400</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50">
+        <v>500</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51">
+        <v>600</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52">
+        <v>400</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53">
+        <v>150</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54">
+        <v>200</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55">
+        <v>300</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B56">
+        <v>400</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57">
+        <v>500</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58">
+        <v>600</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59">
+        <v>650</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60">
+        <v>300</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61">
+        <v>400</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62">
+        <v>500</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63">
+        <v>600</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64">
+        <v>700</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65">
+        <v>400</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B66">
+        <v>500</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67">
+        <v>600</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B68">
+        <v>700</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B69">
+        <v>750</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70">
+        <v>250</v>
+      </c>
+      <c r="C70" s="2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71">
+        <v>300</v>
+      </c>
+      <c r="C71" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72">
+        <v>400</v>
+      </c>
+      <c r="C72" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73">
+        <v>500</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74">
+        <v>600</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75">
+        <v>700</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B76">
+        <v>350</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B77">
+        <v>400</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B78">
+        <v>500</v>
+      </c>
+      <c r="C78" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B79">
+        <v>600</v>
+      </c>
+      <c r="C79" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B80">
+        <v>700</v>
+      </c>
+      <c r="C80" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B81">
+        <v>750</v>
+      </c>
+      <c r="C81" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B82">
+        <v>400</v>
+      </c>
+      <c r="C82" s="2">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B83">
+        <v>450</v>
+      </c>
+      <c r="C83" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B84">
+        <v>500</v>
+      </c>
+      <c r="C84" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B85">
+        <v>600</v>
+      </c>
+      <c r="C85" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B86">
+        <v>350</v>
+      </c>
+      <c r="C86" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B87">
+        <v>400</v>
+      </c>
+      <c r="C87" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B88">
+        <v>400</v>
+      </c>
+      <c r="C88" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B89">
+        <v>450</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B90">
+        <v>500</v>
+      </c>
+      <c r="C90" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B91">
+        <v>600</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B92">
+        <v>700</v>
+      </c>
+      <c r="C92" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B93">
+        <v>300</v>
+      </c>
+      <c r="C93" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B94">
+        <v>250</v>
+      </c>
+      <c r="C94" s="2">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B95">
+        <v>300</v>
+      </c>
+      <c r="C95" s="2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B96">
+        <v>400</v>
+      </c>
+      <c r="C96" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B97">
+        <v>500</v>
+      </c>
+      <c r="C97" s="2">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B98">
+        <v>600</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B99">
+        <v>300</v>
+      </c>
+      <c r="C99" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B100">
+        <v>400</v>
+      </c>
+      <c r="C100" s="2">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B101">
+        <v>500</v>
+      </c>
+      <c r="C101" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B102">
+        <v>600</v>
+      </c>
+      <c r="C102" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B103">
+        <v>700</v>
+      </c>
+      <c r="C103" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B104">
+        <v>800</v>
+      </c>
+      <c r="C104" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B105">
+        <v>450</v>
+      </c>
+      <c r="C105" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B106">
+        <v>500</v>
+      </c>
+      <c r="C106" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B107">
+        <v>600</v>
+      </c>
+      <c r="C107" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B108">
+        <v>650</v>
+      </c>
+      <c r="C108" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B109">
+        <v>700</v>
+      </c>
+      <c r="C109" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B110">
+        <v>350</v>
+      </c>
+      <c r="C110" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B111">
+        <v>400</v>
+      </c>
+      <c r="C111" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B112">
+        <v>350</v>
+      </c>
+      <c r="C112" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B113">
+        <v>400</v>
+      </c>
+      <c r="C113" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B114">
+        <v>250</v>
+      </c>
+      <c r="C114" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B115">
+        <v>300</v>
+      </c>
+      <c r="C115" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B116">
+        <v>400</v>
+      </c>
+      <c r="C116" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B117">
+        <v>500</v>
+      </c>
+      <c r="C117" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B118">
+        <v>600</v>
+      </c>
+      <c r="C118" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B119">
+        <v>350</v>
+      </c>
+      <c r="C119" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B120">
+        <v>400</v>
+      </c>
+      <c r="C120" s="2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B121">
+        <v>500</v>
+      </c>
+      <c r="C121" s="2">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B122">
+        <v>600</v>
+      </c>
+      <c r="C122" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B123">
+        <v>250</v>
+      </c>
+      <c r="C123" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>40</v>
+      </c>
+      <c r="B124">
+        <v>300</v>
+      </c>
+      <c r="C124" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>41</v>
+      </c>
+      <c r="B125">
+        <v>450</v>
+      </c>
+      <c r="C125" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>